<commit_message>
Major modifications for LCA and TEA results
</commit_message>
<xml_diff>
--- a/exposan/enviroloo/data/impact_items.xlsx
+++ b/exposan/enviroloo/data/impact_items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minim\OneDrive\Documents\GitHub\EXPOsan\exposan\enviroloo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\TANG\Documents\GitHub\EXPOsan\exposan\enviroloo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2D507C-7E50-4725-835D-46B90EB4330B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA9CAC6-3BDE-4B45-B887-72F1F8B8EE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10848" yWindow="0" windowWidth="12660" windowHeight="12216" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -294,11 +294,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -317,7 +317,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -331,7 +331,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -341,26 +341,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -383,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -413,8 +400,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,18 +708,18 @@
   </sheetPr>
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>55</v>
       </c>
@@ -750,7 +735,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
@@ -758,7 +743,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
@@ -766,7 +751,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
@@ -774,7 +759,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>60</v>
       </c>
@@ -782,7 +767,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>68</v>
       </c>
@@ -790,7 +775,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
@@ -798,7 +783,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -806,7 +791,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -814,7 +799,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -822,7 +807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -830,7 +815,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -838,7 +823,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -846,7 +831,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -854,7 +839,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -862,7 +847,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -870,7 +855,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -878,7 +863,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -886,7 +871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -894,7 +879,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -902,7 +887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -910,7 +895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" customHeight="1">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -918,7 +903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18.75" customHeight="1">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -926,7 +911,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18.75" customHeight="1">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -934,7 +919,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18.75" customHeight="1">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -942,7 +927,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -950,7 +935,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="18.75" customHeight="1">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -958,7 +943,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18.75" customHeight="1">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -966,91 +951,91 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.4">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.4">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.4">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.4">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.4">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.4">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.4">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.4">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.4">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.4">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1067,21 +1052,21 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A40"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="12"/>
+    <col min="1" max="1" width="26.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -1127,7 +1112,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -1150,7 +1135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -1173,7 +1158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -1196,7 +1181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -1219,7 +1204,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1227,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -1265,7 +1250,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1311,7 +1296,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -1334,7 +1319,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -1357,7 +1342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -1380,7 +1365,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1403,7 +1388,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -1426,7 +1411,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -1449,7 +1434,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -1472,7 +1457,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -1495,7 +1480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -1518,7 +1503,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -1541,7 +1526,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -1564,7 +1549,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -1587,7 +1572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -1610,7 +1595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1635,7 +1620,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -1658,7 +1643,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -1681,7 +1666,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1704,7 +1689,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1727,7 +1712,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -1750,274 +1735,274 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.6">
-      <c r="A30" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="7">
         <v>8.8474600327818393</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="7">
         <v>7.9627140295036556</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="7">
         <v>9.732206036060024</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.6">
-      <c r="A31" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="7">
         <v>4.3790218750000003</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="7">
         <v>3.9411196875000005</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="7">
         <v>4.8169240625000009</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.6">
-      <c r="A32" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="7">
         <v>4.0684475872536101</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="7">
         <f t="shared" ref="D32" si="0">C32*0.9</f>
         <v>3.6616028285282494</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="7">
         <f t="shared" ref="E32" si="1">C32*1.1</f>
         <v>4.4752923459789713</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="7">
         <v>268.39624049999998</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="7">
         <f>C33*0.9</f>
         <v>241.55661644999998</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="7">
         <f>C33*1.1</f>
         <v>295.23586454999997</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6">
-      <c r="A34" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="7">
         <v>18.560989660000001</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="7">
         <f t="shared" ref="D34:D38" si="2">C34*0.9</f>
         <v>16.704890693999999</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="7">
         <f t="shared" ref="E34:E38" si="3">C34*1.1</f>
         <v>20.417088626000002</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6">
-      <c r="A35" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="7">
         <v>26.79636172</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="7">
         <f t="shared" si="2"/>
         <v>24.116725548000002</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="7">
         <f t="shared" si="3"/>
         <v>29.475997892000002</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="F35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.6">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="7">
         <v>640.94971980000003</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="7">
         <f t="shared" si="2"/>
         <v>576.85474782000006</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="7">
         <f t="shared" si="3"/>
         <v>705.04469178000011</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="F36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.6">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="7">
         <v>64.485798299999999</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="7">
         <f t="shared" si="2"/>
         <v>58.037218469999999</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="7">
         <f t="shared" si="3"/>
         <v>70.934378129999999</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.6">
-      <c r="A38" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="7">
         <v>4.5353009950000001</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="7">
         <f t="shared" si="2"/>
         <v>4.0817708955000001</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="7">
         <f t="shared" si="3"/>
         <v>4.9888310945000001</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.6">
-      <c r="A39" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="7">
         <v>7.0524620000000002</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="7">
         <f t="shared" ref="D39:D40" si="4">C39*0.9</f>
         <v>6.3472158000000007</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="7">
         <f t="shared" ref="E39:E40" si="5">C39*1.1</f>
         <v>7.7577082000000006</v>
       </c>
-      <c r="F39" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.6">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="7">
         <v>6.2828470000000003</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="7">
         <f t="shared" si="4"/>
         <v>5.6545623000000003</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="7">
         <f t="shared" si="5"/>
         <v>6.9111317000000012</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="F40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2034,21 +2019,21 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:G35"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +2057,7 @@
       </c>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -2098,7 +2083,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -2124,7 +2109,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -2150,7 +2135,7 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -2176,7 +2161,7 @@
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -2202,7 +2187,7 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -2228,7 +2213,7 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -2254,7 +2239,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -2278,7 +2263,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -2302,7 +2287,7 @@
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -2326,7 +2311,7 @@
       </c>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -2350,7 +2335,7 @@
       </c>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -2374,7 +2359,7 @@
       </c>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -2398,7 +2383,7 @@
       </c>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -2422,7 +2407,7 @@
       </c>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1">
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -2446,7 +2431,7 @@
       </c>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -2470,7 +2455,7 @@
       </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2494,7 +2479,7 @@
       </c>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1">
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -2518,7 +2503,7 @@
       </c>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1">
+    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -2542,7 +2527,7 @@
       </c>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1">
+    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -2566,7 +2551,7 @@
       </c>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1">
+    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -2590,7 +2575,7 @@
       </c>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1">
+    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -2614,7 +2599,7 @@
       </c>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1">
+    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -2640,7 +2625,7 @@
       </c>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1">
+    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -2664,7 +2649,7 @@
       </c>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1">
+    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -2688,7 +2673,7 @@
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1">
+    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -2712,7 +2697,7 @@
       </c>
       <c r="H27" s="12"/>
     </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1">
+    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -2736,7 +2721,7 @@
       </c>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1">
+    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -2760,278 +2745,278 @@
       </c>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:8" ht="14.4">
-      <c r="A30" t="s">
+    <row r="30" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="B30" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="7">
         <v>0.30296211312539301</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="7">
         <f t="shared" ref="D30:D31" si="2">C30*0.9</f>
         <v>0.27266590181285372</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="7">
         <f t="shared" ref="E30:E31" si="3">C30*1.1</f>
         <v>0.33325832443793235</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="15">
+      <c r="B31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="7">
         <v>1.9420648277268783E-2</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="7">
         <f t="shared" si="2"/>
         <v>1.7478583449541906E-2</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="7">
         <f t="shared" si="3"/>
         <v>2.1362713104995663E-2</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.4">
-      <c r="A32" t="s">
+    <row r="32" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="15">
+      <c r="B32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="7">
         <v>7.4320484114979005E-2</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="7">
         <f t="shared" ref="D32:D35" si="4">C32*0.9</f>
         <v>6.6888435703481103E-2</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="7">
         <f t="shared" ref="E32:E35" si="5">C32*1.1</f>
         <v>8.1752532526476906E-2</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.4">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="15">
+      <c r="B33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="7">
         <v>1.1374107377821401</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="7">
         <f t="shared" si="4"/>
         <v>1.023669664003926</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="7">
         <f t="shared" si="5"/>
         <v>1.2511518115603542</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.4">
-      <c r="A34" t="s">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="15">
+      <c r="B34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7">
         <v>9.9859563940134302E-2</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="7">
         <f t="shared" si="4"/>
         <v>8.9873607546120879E-2</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="7">
         <f t="shared" si="5"/>
         <v>0.10984552033414774</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6">
-      <c r="A35" t="s">
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="15">
+      <c r="B35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="7">
         <v>0.12050920688542401</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="7">
         <f t="shared" si="4"/>
         <v>0.10845828619688161</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="7">
         <f t="shared" si="5"/>
         <v>0.13256012757396643</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="16" t="s">
+      <c r="F35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.6">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="15">
+      <c r="B36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="7">
         <v>2.8262379633255601</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="7">
         <f t="shared" ref="D36:D38" si="6">C36*0.9</f>
         <v>2.5436141669930041</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="7">
         <f t="shared" ref="E36:E38" si="7">C36*1.1</f>
         <v>3.1088617596581165</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="16" t="s">
+      <c r="F36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.4">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="15">
+      <c r="B37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7">
         <v>0.30296211312539301</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="7">
         <f t="shared" si="6"/>
         <v>0.27266590181285372</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="7">
         <f t="shared" si="7"/>
         <v>0.33325832443793235</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.4">
-      <c r="A38" t="s">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="15">
+      <c r="B38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="7">
         <v>2.1307106118144098E-2</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="7">
         <f t="shared" si="6"/>
         <v>1.9176395506329689E-2</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="7">
         <f t="shared" si="7"/>
         <v>2.3437816729958511E-2</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.4">
-      <c r="A39" t="s">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="15">
+      <c r="B39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="7">
         <v>2.50035291316336E-2</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="7">
         <f t="shared" ref="D39:D40" si="8">C39*0.9</f>
         <v>2.2503176218470242E-2</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="7">
         <f t="shared" ref="E39:E40" si="9">C39*1.1</f>
         <v>2.7503882044796962E-2</v>
       </c>
-      <c r="F39" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.6">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="15">
+      <c r="B40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="7">
         <v>2.50035291316336E-2</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="7">
         <f t="shared" si="8"/>
         <v>2.2503176218470242E-2</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="7">
         <f t="shared" si="9"/>
         <v>2.7503882044796962E-2</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="16" t="s">
+      <c r="F40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3048,21 +3033,21 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:G40"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3085,7 +3070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -3110,7 +3095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -3135,7 +3120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -3160,7 +3145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -3185,7 +3170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -3210,7 +3195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>68</v>
       </c>
@@ -3235,7 +3220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -3260,7 +3245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -3283,7 +3268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -3306,7 +3291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -3329,7 +3314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -3352,7 +3337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -3375,7 +3360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -3398,7 +3383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -3421,7 +3406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -3444,7 +3429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -3467,7 +3452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -3492,7 +3477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -3515,7 +3500,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -3538,7 +3523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -3561,7 +3546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -3584,7 +3569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -3607,7 +3592,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -3632,7 +3617,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -3655,7 +3640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -3678,7 +3663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -3701,7 +3686,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -3724,7 +3709,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -3747,278 +3732,278 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.4">
-      <c r="A30" t="s">
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="B30" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="7">
         <v>14.15675868232</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="7">
         <f t="shared" ref="D30:D40" si="2">C30*0.9</f>
         <v>12.741082814087999</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="7">
         <f t="shared" ref="E30:E40" si="3">C30*1.1</f>
         <v>15.572434550552002</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="14.4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="15">
+      <c r="B31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="7">
         <v>0.90748453091794867</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="7">
         <f t="shared" si="2"/>
         <v>0.81673607782615387</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="7">
         <f t="shared" si="3"/>
         <v>0.99823298400974358</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.4">
-      <c r="A32" t="s">
+    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="15">
+      <c r="B32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="7">
         <v>1.40205409119104</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="7">
         <f t="shared" si="2"/>
         <v>1.2618486820719359</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="7">
         <f t="shared" si="3"/>
         <v>1.542259500310144</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.4">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="15">
+      <c r="B33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="7">
         <v>19.661164093733099</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="7">
         <f t="shared" si="2"/>
         <v>17.695047684359789</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="7">
         <f t="shared" si="3"/>
         <v>21.627280503106409</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.4">
-      <c r="A34" t="s">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="15">
+      <c r="B34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7">
         <v>10.064333355825401</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="7">
         <f t="shared" si="2"/>
         <v>9.0579000202428617</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="7">
         <f t="shared" si="3"/>
         <v>11.070766691407941</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6">
-      <c r="A35" t="s">
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="15">
+      <c r="B35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="7">
         <v>5.1980994597015604</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="7">
         <f t="shared" si="2"/>
         <v>4.6782895137314044</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="7">
         <f t="shared" si="3"/>
         <v>5.7179094056717172</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="16" t="s">
+      <c r="F35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.6">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="15">
+      <c r="B36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="7">
         <v>154.345721658065</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="7">
         <f t="shared" si="2"/>
         <v>138.91114949225852</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="7">
         <f t="shared" si="3"/>
         <v>169.78029382387152</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="16" t="s">
+      <c r="F36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.4">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="15">
+      <c r="B37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7">
         <v>14.15675868232</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="7">
         <f t="shared" si="2"/>
         <v>12.741082814087999</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="7">
         <f t="shared" si="3"/>
         <v>15.572434550552002</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.4">
-      <c r="A38" t="s">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="15">
+      <c r="B38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="7">
         <v>1.7020829880008299</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="7">
         <f t="shared" si="2"/>
         <v>1.5318746892007469</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="7">
         <f t="shared" si="3"/>
         <v>1.8722912868009129</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.4">
-      <c r="A39" t="s">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="15">
+      <c r="B39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="7">
         <v>1.08010771409159</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="7">
         <f t="shared" si="2"/>
         <v>0.97209694268243108</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="7">
         <f t="shared" si="3"/>
         <v>1.1881184855007492</v>
       </c>
-      <c r="F39" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.6">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="15">
+      <c r="B40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="7">
         <v>1.08010771409159</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="7">
         <f t="shared" si="2"/>
         <v>0.97209694268243108</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="7">
         <f t="shared" si="3"/>
         <v>1.1881184855007492</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="16" t="s">
+      <c r="F40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4035,20 +4020,20 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:G40"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4071,7 +4056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -4096,7 +4081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -4121,7 +4106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -4146,7 +4131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1">
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -4171,7 +4156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1">
+    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -4196,7 +4181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -4221,7 +4206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -4246,7 +4231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1">
+    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -4269,7 +4254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -4292,7 +4277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -4315,7 +4300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1">
+    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -4338,7 +4323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1">
+    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -4361,7 +4346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1">
+    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -4384,7 +4369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1">
+    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -4407,7 +4392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1">
+    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -4433,7 +4418,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -4456,7 +4441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1">
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -4479,7 +4464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1">
+    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -4502,7 +4487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1">
+    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -4525,7 +4510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1">
+    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -4548,7 +4533,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1">
+    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -4571,7 +4556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1">
+    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -4594,7 +4579,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="19.5" customHeight="1">
+    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -4619,7 +4604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19.5" customHeight="1">
+    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -4642,7 +4627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="19.5" customHeight="1">
+    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -4665,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="19.5" customHeight="1">
+    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -4688,7 +4673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="19.5" customHeight="1">
+    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -4711,7 +4696,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="19.5" customHeight="1">
+    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -4734,278 +4719,278 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.6">
-      <c r="A30" t="s">
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="B30" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="7">
         <v>8.3066274332224399</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="7">
         <f t="shared" ref="D30:D40" si="2">C30*0.9</f>
         <v>7.4759646899001959</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="7">
         <f t="shared" ref="E30:E40" si="3">C30*1.1</f>
         <v>9.1372901765446848</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="16" t="s">
+      <c r="F30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="14.4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="15">
+      <c r="B31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="7">
         <v>0.53247611751425894</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="7">
         <f t="shared" si="2"/>
         <v>0.47922850576283305</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="7">
         <f t="shared" si="3"/>
         <v>0.58572372926568483</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.6">
-      <c r="A32" t="s">
+    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="15">
+      <c r="B32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="7">
         <v>0.59132638892400702</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="7">
         <f t="shared" si="2"/>
         <v>0.53219375003160629</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="7">
         <f t="shared" si="3"/>
         <v>0.65045902781640774</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="16" t="s">
+      <c r="F32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="15">
+      <c r="B33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="7">
         <v>12.2640088136837</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="7">
         <f t="shared" si="2"/>
         <v>11.03760793231533</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="7">
         <f t="shared" si="3"/>
         <v>13.490409695052072</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="16" t="s">
+      <c r="F33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6">
-      <c r="A34" t="s">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="15">
+      <c r="B34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7">
         <v>3.8648818235700597</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="7">
         <f t="shared" si="2"/>
         <v>3.4783936412130538</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="7">
         <f t="shared" si="3"/>
         <v>4.2513700059270656</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="16" t="s">
+      <c r="F34" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6">
-      <c r="A35" t="s">
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="15">
+      <c r="B35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="7">
         <v>2.8962775801561298</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="7">
         <f t="shared" si="2"/>
         <v>2.606649822140517</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="7">
         <f t="shared" si="3"/>
         <v>3.185905338171743</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="16" t="s">
+      <c r="F35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.4">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="15">
+      <c r="B36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="7">
         <v>62.577397919048998</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="7">
         <f t="shared" si="2"/>
         <v>56.319658127144102</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="7">
         <f t="shared" si="3"/>
         <v>68.835137710953902</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="F36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.4">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="15">
+      <c r="B37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7">
         <v>8.3066274332224399</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="7">
         <f t="shared" si="2"/>
         <v>7.4759646899001959</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="7">
         <f t="shared" si="3"/>
         <v>9.1372901765446848</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.6">
-      <c r="A38" t="s">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="15">
+      <c r="B38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="7">
         <v>3.1480737476934801</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="7">
         <f t="shared" si="2"/>
         <v>2.8332663729241321</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="7">
         <f t="shared" si="3"/>
         <v>3.4628811224628286</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="16" t="s">
+      <c r="F38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.4">
-      <c r="A39" t="s">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="15">
+      <c r="B39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="7">
         <v>1.1964417886707701</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="7">
         <f t="shared" si="2"/>
         <v>1.0767976098036931</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="7">
         <f t="shared" si="3"/>
         <v>1.3160859675378471</v>
       </c>
-      <c r="F39" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.6">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="15">
+      <c r="B40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="7">
         <v>1.1964417886707701</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="7">
         <f t="shared" si="2"/>
         <v>1.0767976098036931</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="7">
         <f t="shared" si="3"/>
         <v>1.3160859675378471</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="16" t="s">
+      <c r="F40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="12" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added electricity grid share to all
</commit_message>
<xml_diff>
--- a/exposan/enviroloo/data/impact_items.xlsx
+++ b/exposan/enviroloo/data/impact_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\TANG\Documents\GitHub\EXPOsan\exposan\enviroloo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabhpuri/Documents/Github/EXPOsan/exposan/enviroloo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA9CAC6-3BDE-4B45-B887-72F1F8B8EE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C399C7-8782-4348-976E-DF237632B355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>LithiumBattery</t>
+  </si>
+  <si>
+    <t>GridElectricity</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -317,7 +320,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -331,7 +334,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -706,20 +709,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +730,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>55</v>
       </c>
@@ -735,7 +738,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
@@ -743,7 +746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
@@ -751,7 +754,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
@@ -759,7 +762,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>60</v>
       </c>
@@ -767,7 +770,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>68</v>
       </c>
@@ -775,7 +778,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
@@ -783,7 +786,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -791,7 +794,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -799,7 +802,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -807,7 +810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -815,7 +818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -823,7 +826,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -831,7 +834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -839,7 +842,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -847,7 +850,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -855,7 +858,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -863,7 +866,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -871,7 +874,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -879,7 +882,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -887,7 +890,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -895,7 +898,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -903,7 +906,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -911,7 +914,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -919,7 +922,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -927,7 +930,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -935,7 +938,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -943,7 +946,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -951,7 +954,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
@@ -959,7 +962,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
@@ -967,7 +970,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -975,7 +978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -983,7 +986,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
@@ -991,7 +994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
@@ -1031,11 +1034,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
       <c r="B40" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1050,23 +1061,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.54296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="12"/>
+    <col min="1" max="1" width="26.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -1112,7 +1123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -1135,7 +1146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -1158,7 +1169,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -1181,7 +1192,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -1204,7 +1215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1227,7 +1238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -1250,7 +1261,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -1273,7 +1284,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -1296,7 +1307,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -1319,7 +1330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -1342,7 +1353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -1365,7 +1376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1399,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -1411,7 +1422,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -1434,7 +1445,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -1457,7 +1468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -1480,7 +1491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -1503,7 +1514,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -1526,7 +1537,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -1549,7 +1560,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -1572,7 +1583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -1595,7 +1606,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1620,7 +1631,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -1643,7 +1654,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -1666,7 +1677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1689,7 +1700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1712,7 +1723,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -1735,7 +1746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
@@ -1758,7 +1769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
@@ -1781,7 +1792,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -1806,7 +1817,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -1831,7 +1842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
@@ -1856,7 +1867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -1881,7 +1892,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
@@ -1906,7 +1917,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
@@ -1931,7 +1942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
@@ -1956,7 +1967,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
@@ -1967,11 +1978,11 @@
         <v>7.0524620000000002</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" ref="D39:D40" si="4">C39*0.9</f>
+        <f t="shared" ref="D39:D41" si="4">C39*0.9</f>
         <v>6.3472158000000007</v>
       </c>
       <c r="E39" s="7">
-        <f t="shared" ref="E39:E40" si="5">C39*1.1</f>
+        <f t="shared" ref="E39:E41" si="5">C39*1.1</f>
         <v>7.7577082000000006</v>
       </c>
       <c r="F39" s="12" t="s">
@@ -1981,7 +1992,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
@@ -2003,6 +2014,30 @@
         <v>9</v>
       </c>
       <c r="G40" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="5"/>
+        <v>1.034</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2023,17 +2058,17 @@
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2092,7 @@
       </c>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -2083,7 +2118,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -2109,7 +2144,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -2135,7 +2170,7 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -2161,7 +2196,7 @@
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -2187,7 +2222,7 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -2213,7 +2248,7 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -2239,7 +2274,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -2263,7 +2298,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -2287,7 +2322,7 @@
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -2311,7 +2346,7 @@
       </c>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -2335,7 +2370,7 @@
       </c>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -2359,7 +2394,7 @@
       </c>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -2383,7 +2418,7 @@
       </c>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -2407,7 +2442,7 @@
       </c>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -2431,7 +2466,7 @@
       </c>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -2455,7 +2490,7 @@
       </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2479,7 +2514,7 @@
       </c>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -2503,7 +2538,7 @@
       </c>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -2527,7 +2562,7 @@
       </c>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -2551,7 +2586,7 @@
       </c>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -2575,7 +2610,7 @@
       </c>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -2599,7 +2634,7 @@
       </c>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -2625,7 +2660,7 @@
       </c>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -2649,7 +2684,7 @@
       </c>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -2673,7 +2708,7 @@
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -2697,7 +2732,7 @@
       </c>
       <c r="H27" s="12"/>
     </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -2721,7 +2756,7 @@
       </c>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -2745,7 +2780,7 @@
       </c>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
@@ -2770,7 +2805,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
@@ -2795,7 +2830,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -2820,7 +2855,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -2845,7 +2880,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
@@ -2870,7 +2905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -2895,7 +2930,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
@@ -2920,7 +2955,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
@@ -2945,7 +2980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
@@ -2970,7 +3005,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
@@ -2995,7 +3030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
@@ -3037,17 +3072,17 @@
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3070,7 +3105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -3095,7 +3130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -3120,7 +3155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -3145,7 +3180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -3170,7 +3205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -3195,7 +3230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>68</v>
       </c>
@@ -3220,7 +3255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -3245,7 +3280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -3268,7 +3303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -3291,7 +3326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -3314,7 +3349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -3337,7 +3372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -3360,7 +3395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -3383,7 +3418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -3406,7 +3441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -3429,7 +3464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -3452,7 +3487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -3477,7 +3512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -3500,7 +3535,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -3523,7 +3558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -3546,7 +3581,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -3569,7 +3604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -3592,7 +3627,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -3617,7 +3652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -3640,7 +3675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -3663,7 +3698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -3686,7 +3721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -3709,7 +3744,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -3732,7 +3767,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
@@ -3757,7 +3792,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
@@ -3782,7 +3817,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -3807,7 +3842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -3832,7 +3867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
@@ -3857,7 +3892,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -3882,7 +3917,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
@@ -3907,7 +3942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
@@ -3932,7 +3967,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
@@ -3957,7 +3992,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
@@ -3982,7 +4017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>82</v>
       </c>
@@ -4024,16 +4059,16 @@
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4056,7 +4091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -4081,7 +4116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -4106,7 +4141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -4131,7 +4166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -4156,7 +4191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
@@ -4181,7 +4216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -4206,7 +4241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>61</v>
       </c>
@@ -4231,7 +4266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -4254,7 +4289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>69</v>
       </c>
@@ -4277,7 +4312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -4300,7 +4335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
@@ -4323,7 +4358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>63</v>
       </c>
@@ -4346,7 +4381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -4369,7 +4404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
@@ -4392,7 +4427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
@@ -4418,7 +4453,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -4441,7 +4476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -4464,7 +4499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -4487,7 +4522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -4510,7 +4545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -4533,7 +4568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>25</v>
       </c>
@@ -4556,7 +4591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>27</v>
       </c>
@@ -4579,7 +4614,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -4604,7 +4639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -4627,7 +4662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -4650,7 +4685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -4673,7 +4708,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -4696,7 +4731,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>36</v>
       </c>
@@ -4719,7 +4754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>70</v>
       </c>
@@ -4744,7 +4779,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>71</v>
       </c>
@@ -4769,7 +4804,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -4794,7 +4829,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -4819,7 +4854,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
@@ -4844,7 +4879,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -4869,7 +4904,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>78</v>
       </c>
@@ -4894,7 +4929,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
@@ -4919,7 +4954,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>80</v>
       </c>
@@ -4944,7 +4979,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
@@ -4969,7 +5004,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>82</v>
       </c>

</xml_diff>